<commit_message>
glyph update, new tags, circle data fixes
</commit_message>
<xml_diff>
--- a/events/misc 420 - 504.xlsx
+++ b/events/misc 420 - 504.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Projects\GitHub\whimdig\events\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="209">
   <si>
     <t>The Copper Hog</t>
   </si>
@@ -631,16 +636,28 @@
   </si>
   <si>
     <t>5/2/2015 11:00pm</t>
+  </si>
+  <si>
+    <t>theatre</t>
+  </si>
+  <si>
+    <t>alcohol, music</t>
+  </si>
+  <si>
+    <t>alcohol, games</t>
+  </si>
+  <si>
+    <t>alcohol, funny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,6 +707,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -736,7 +761,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -768,9 +793,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -802,6 +828,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -977,23 +1004,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1101,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1093,7 +1121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1113,7 +1141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1133,7 +1161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1156,7 +1184,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1179,7 +1207,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1202,7 +1230,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1222,7 +1250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1242,7 +1270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1262,7 +1290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1282,7 +1310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1305,7 +1333,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1328,7 +1356,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1351,7 +1379,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1371,7 +1399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1394,7 +1422,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1414,7 +1442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1434,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1454,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1477,7 +1505,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1500,7 +1528,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -1523,7 +1551,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -1546,7 +1574,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -1566,7 +1594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1586,7 +1614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -1606,7 +1634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1626,7 +1654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1646,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -1669,7 +1697,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -1689,7 +1717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1709,7 +1737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -1729,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -1749,7 +1777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -1769,7 +1797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -1789,7 +1817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -1809,7 +1837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>144</v>
       </c>
@@ -1829,7 +1857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>144</v>
       </c>
@@ -1849,7 +1877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>144</v>
       </c>
@@ -1872,7 +1900,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>144</v>
       </c>
@@ -1892,7 +1920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -1912,7 +1940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -1932,7 +1960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>163</v>
       </c>
@@ -1952,7 +1980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>163</v>
       </c>
@@ -1972,7 +2000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1">
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>163</v>
       </c>
@@ -1992,7 +2020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1">
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>163</v>
       </c>
@@ -2012,10 +2040,13 @@
         <v>5</v>
       </c>
       <c r="G49" t="s">
+        <v>206</v>
+      </c>
+      <c r="H49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1">
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>163</v>
       </c>
@@ -2035,10 +2066,13 @@
         <v>6</v>
       </c>
       <c r="G50" t="s">
+        <v>206</v>
+      </c>
+      <c r="H50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1">
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>163</v>
       </c>
@@ -2058,10 +2092,13 @@
         <v>5</v>
       </c>
       <c r="G51" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1">
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>163</v>
       </c>
@@ -2081,10 +2118,13 @@
         <v>6</v>
       </c>
       <c r="G52" t="s">
+        <v>206</v>
+      </c>
+      <c r="H52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1">
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>163</v>
       </c>
@@ -2104,10 +2144,13 @@
         <v>6</v>
       </c>
       <c r="G53" t="s">
+        <v>206</v>
+      </c>
+      <c r="H53" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1">
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -2127,10 +2170,13 @@
         <v>6</v>
       </c>
       <c r="G54" t="s">
+        <v>208</v>
+      </c>
+      <c r="H54" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1">
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>193</v>
       </c>
@@ -2149,8 +2195,11 @@
       <c r="F55" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1">
+      <c r="G55" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -2169,8 +2218,11 @@
       <c r="F56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1">
+      <c r="G56" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>193</v>
       </c>
@@ -2189,8 +2241,11 @@
       <c r="F57" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1">
+      <c r="G57" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>193</v>
       </c>
@@ -2209,8 +2264,11 @@
       <c r="F58" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1">
+      <c r="G58" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -2229,8 +2287,11 @@
       <c r="F59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1">
+      <c r="G59" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>193</v>
       </c>
@@ -2249,8 +2310,11 @@
       <c r="F60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15" customHeight="1">
+      <c r="G60" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>193</v>
       </c>
@@ -2269,8 +2333,11 @@
       <c r="F61" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="15" customHeight="1">
+      <c r="G61" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>193</v>
       </c>
@@ -2288,6 +2355,9 @@
       </c>
       <c r="F62" t="s">
         <v>5</v>
+      </c>
+      <c r="G62" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2297,24 +2367,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>